<commit_message>
debut des correction Audit
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Documents\Formation Developpeur\P4_Desseré_Quentin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quent\Documents\Formation Developpeur\P4_Desseré_Quentin\projetmodif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA50E622-FE52-4B09-BF56-956270D1A1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47D1AA6-3C86-4D82-BBFE-F29D15BC2991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Catégorie</t>
   </si>
@@ -78,18 +78,9 @@
     <t>mentionner webdesign</t>
   </si>
   <si>
-    <t>utiliser mots clés d'intention</t>
-  </si>
-  <si>
-    <t>utiliser mots clés de marque</t>
-  </si>
-  <si>
     <t>https://kwfinder.com/</t>
   </si>
   <si>
-    <t>Seo</t>
-  </si>
-  <si>
     <t>page 2 sans nom</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
     <t>pas de balise title</t>
   </si>
   <si>
-    <t>H2 avant H3</t>
-  </si>
-  <si>
     <t>page 2 sans keywords</t>
   </si>
   <si>
@@ -139,13 +127,126 @@
   </si>
   <si>
     <t>revoir le code css</t>
+  </si>
+  <si>
+    <t>accessibilité</t>
+  </si>
+  <si>
+    <t>contrast error</t>
+  </si>
+  <si>
+    <t>liens footer trop clair</t>
+  </si>
+  <si>
+    <t>diminuer luminosité</t>
+  </si>
+  <si>
+    <r>
+      <t>couleur : #171717</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF202124"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>mauvaise pratique</t>
+  </si>
+  <si>
+    <t>supprimer la section</t>
+  </si>
+  <si>
+    <t>section supprimée</t>
+  </si>
+  <si>
+    <t>p ligne 225 trop clair</t>
+  </si>
+  <si>
+    <t>"Contact" lignes 74/ 212 trop clair</t>
+  </si>
+  <si>
+    <t>couleur : #1A1A1A</t>
+  </si>
+  <si>
+    <t>titre h2 trop sombre</t>
+  </si>
+  <si>
+    <t>augmenter luminosité</t>
+  </si>
+  <si>
+    <t>couleur : #FBE8DF</t>
+  </si>
+  <si>
+    <t>H3 avant H2</t>
+  </si>
+  <si>
+    <t>liens reseaux sociaux à remplir</t>
+  </si>
+  <si>
+    <t>actuellement, liens vers l'index</t>
+  </si>
+  <si>
+    <t>changer les liens</t>
+  </si>
+  <si>
+    <t>alt images similaires</t>
+  </si>
+  <si>
+    <t>paragraphe caché avec des liens(logo) puis dans la page</t>
+  </si>
+  <si>
+    <t>nom non pertinant</t>
+  </si>
+  <si>
+    <t>renommer "contact"</t>
+  </si>
+  <si>
+    <t>wave webaim</t>
+  </si>
+  <si>
+    <t>lighthouse</t>
+  </si>
+  <si>
+    <t>pas de description dans meta</t>
+  </si>
+  <si>
+    <t>remplir la description</t>
+  </si>
+  <si>
+    <t>mettre quelque chose de cohérent</t>
+  </si>
+  <si>
+    <t>font-size&lt;12px</t>
+  </si>
+  <si>
+    <t>&lt;12 px pas bien</t>
+  </si>
+  <si>
+    <t>mettre size à 12px</t>
+  </si>
+  <si>
+    <t>liens partenaires trop proches</t>
+  </si>
+  <si>
+    <t>espacer les liens</t>
+  </si>
+  <si>
+    <t>ajouter un padding-bottom</t>
+  </si>
+  <si>
+    <t>.col-sm-4 li : padding-bottom : 5px;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -175,6 +276,23 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -210,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,6 +336,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,19 +557,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="41.88671875" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
+    <col min="2" max="2" width="54.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" customWidth="1"/>
     <col min="4" max="4" width="27.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23" customWidth="1"/>
+    <col min="5" max="5" width="35.77734375" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" customWidth="1"/>
     <col min="7" max="26" width="10.5546875" customWidth="1"/>
   </cols>
@@ -496,7 +620,7 @@
       </c>
       <c r="E2" s="4"/>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -515,6 +639,9 @@
       <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -526,44 +653,66 @@
       <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="F4" s="5" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" s="4" t="s">
+      <c r="A6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -571,8 +720,8 @@
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
+      <c r="B10" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="4"/>
     </row>
@@ -581,29 +730,43 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -611,52 +774,172 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="E18" t="s">
         <v>28</v>
       </c>
-      <c r="D15" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
+      <c r="E19" t="s">
         <v>31</v>
       </c>
-      <c r="E16" t="s">
+    </row>
+    <row r="20" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="6"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E17" t="s">
+      <c r="C24" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E24" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="E27" s="7"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1625,8 +1908,12 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>